<commit_message>
Deleted the Engine effects From the lap time
</commit_message>
<xml_diff>
--- a/OpenVEHICLE tmp.xlsx
+++ b/OpenVEHICLE tmp.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Google Drive\Youtube VD\Release\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quinh\OneDrive\Documents\Open Lap Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1730960B-4A09-4B06-9F7B-3B14A3516D37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8745" windowHeight="12405"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="68">
   <si>
     <t>General</t>
   </si>
@@ -174,69 +175,12 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>Engine</t>
-  </si>
-  <si>
-    <t>Power Factor Multiplier</t>
-  </si>
-  <si>
-    <t>Thermal Efficiency</t>
-  </si>
-  <si>
-    <t>Fuel Lower Heating Value</t>
-  </si>
-  <si>
-    <t>J/kg</t>
-  </si>
-  <si>
-    <t>Transmission</t>
-  </si>
-  <si>
-    <t>Drive Type</t>
-  </si>
-  <si>
     <t>[Steering Wheel Angle]/[Wheel Angle]</t>
   </si>
   <si>
     <t>[Foot Force Application Point Lever Arm]/[Master Cylinder Lever Arm]</t>
   </si>
   <si>
-    <t>Primary Gear Reduction</t>
-  </si>
-  <si>
-    <t>Final Gear Reduction</t>
-  </si>
-  <si>
-    <t>1st Gear Ratio</t>
-  </si>
-  <si>
-    <t>2nd Gear Ratio</t>
-  </si>
-  <si>
-    <t>3rd Gear Ratio</t>
-  </si>
-  <si>
-    <t>4th Gear Ratio</t>
-  </si>
-  <si>
-    <t>5th Gear Ratio</t>
-  </si>
-  <si>
-    <t>6th Gear Ratio</t>
-  </si>
-  <si>
-    <t>7th Gear Ratio</t>
-  </si>
-  <si>
-    <t>8th Gear Ratio</t>
-  </si>
-  <si>
-    <t>9th Gear Ratio</t>
-  </si>
-  <si>
-    <t>10th Gear Ratio</t>
-  </si>
-  <si>
     <t>Front Aero Distribution</t>
   </si>
   <si>
@@ -246,27 +190,9 @@
     <t>Drag Coefficient CD</t>
   </si>
   <si>
-    <t>Primary Gear Efficiency</t>
-  </si>
-  <si>
-    <t>Final Gear Efficiency</t>
-  </si>
-  <si>
-    <t>Gearbox Efficiency</t>
-  </si>
-  <si>
     <t>Pad Friction Coefficient</t>
   </si>
   <si>
-    <t>Gear Shift Time</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>Only used in dragster mode</t>
-  </si>
-  <si>
     <t>Assumed to be the same on all pads. Recommended value: 0.45</t>
   </si>
   <si>
@@ -285,12 +211,6 @@
     <t>Positive = Lift / Negative = Downforce</t>
   </si>
   <si>
-    <t>Recommended value:  0.90 for bevel gears</t>
-  </si>
-  <si>
-    <t>Recommended value:  0.98 for spur/helical gears</t>
-  </si>
-  <si>
     <t>Assumed to be the same on all tyres. Recommended value: M/4</t>
   </si>
   <si>
@@ -309,19 +229,13 @@
     <t>Assumed to be the same both front and rear.</t>
   </si>
   <si>
-    <t>Recommended value: 0.3 for ICE</t>
-  </si>
-  <si>
-    <t>Recommended value:  4.72E+07 for petrol</t>
-  </si>
-  <si>
-    <t>From crancskaft to Input shaft.</t>
+    <t>Open Wheel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -371,7 +285,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -395,13 +309,45 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -414,10 +360,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -429,10 +375,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -444,10 +390,10 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -459,7 +405,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -474,7 +420,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -489,7 +435,7 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -504,10 +450,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -516,107 +462,12 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -626,7 +477,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -636,67 +487,46 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -715,11 +545,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B3" totalsRowShown="0">
-  <autoFilter ref="A1:B3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B3" totalsRowShown="0">
+  <autoFilter ref="A1:B3" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Engine Speed [rpm]"/>
-    <tableColumn id="2" name="Torque [Nm]"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Engine Speed [rpm]"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Torque [Nm]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -987,11 +817,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C35" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,128 +833,142 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="22" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="10" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="11"/>
+      <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="34"/>
-      <c r="B3" s="12" t="s">
+      <c r="A3" s="24"/>
+      <c r="B3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="14" t="s">
+      <c r="C3" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="15"/>
+      <c r="E3" s="12"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="10" t="s">
+      <c r="C4" s="6">
+        <v>650</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="11"/>
+      <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="34"/>
-      <c r="B5" s="12" t="s">
+      <c r="A5" s="24"/>
+      <c r="B5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="14" t="s">
+      <c r="C5" s="10">
+        <v>45</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="15"/>
+      <c r="E5" s="12"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="19" t="s">
+      <c r="C6" s="15">
+        <v>3000</v>
+      </c>
+      <c r="D6" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="20"/>
+      <c r="E6" s="17"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19" t="s">
+      <c r="C7" s="15">
+        <v>10</v>
+      </c>
+      <c r="D7" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="20" t="s">
-        <v>56</v>
+      <c r="E7" s="17" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="10" t="s">
+      <c r="B8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="6">
+        <v>-4.8</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="11" t="s">
-        <v>85</v>
+      <c r="E8" s="8" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="35"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C9" s="4"/>
+        <v>53</v>
+      </c>
+      <c r="C9" s="4">
+        <v>-1.2</v>
+      </c>
       <c r="D9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="21" t="s">
-        <v>84</v>
+      <c r="E9" s="18" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="35"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="2" t="s">
         <v>20</v>
       </c>
@@ -1134,10 +978,10 @@
       <c r="D10" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="21"/>
+      <c r="E10" s="18"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="35"/>
+      <c r="A11" s="25"/>
       <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
@@ -1147,530 +991,328 @@
       <c r="D11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="21"/>
+      <c r="E11" s="18"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C12" s="4"/>
+        <v>51</v>
+      </c>
+      <c r="C12" s="4">
+        <v>50</v>
+      </c>
       <c r="D12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="21"/>
+      <c r="E12" s="18"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="4"/>
+      <c r="C13" s="4">
+        <v>1</v>
+      </c>
       <c r="D13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="21"/>
+      <c r="E13" s="18"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="34"/>
-      <c r="B14" s="12" t="s">
+      <c r="A14" s="24"/>
+      <c r="B14" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="14" t="s">
+      <c r="C14" s="10">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="D14" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="15" t="s">
-        <v>83</v>
+      <c r="E14" s="12" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="10" t="s">
+      <c r="C15" s="6">
+        <v>250</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="11" t="s">
-        <v>92</v>
+      <c r="E15" s="8" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
+      <c r="A16" s="25"/>
       <c r="B16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="4"/>
+      <c r="C16" s="4">
+        <v>40</v>
+      </c>
       <c r="D16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="21" t="s">
-        <v>92</v>
+      <c r="E16" s="18" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="35"/>
+      <c r="A17" s="25"/>
       <c r="B17" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C17" s="4"/>
+        <v>54</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0.45</v>
+      </c>
       <c r="D17" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="21" t="s">
-        <v>80</v>
+      <c r="E17" s="18" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="35"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="4"/>
+      <c r="C18" s="4">
+        <v>6</v>
+      </c>
       <c r="D18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="21" t="s">
-        <v>92</v>
+      <c r="E18" s="18" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
+      <c r="A19" s="25"/>
       <c r="B19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="4"/>
+      <c r="C19" s="4">
+        <v>40</v>
+      </c>
       <c r="D19" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="21" t="s">
-        <v>92</v>
+      <c r="E19" s="18" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="35"/>
+      <c r="A20" s="25"/>
       <c r="B20" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="4"/>
+      <c r="C20" s="4">
+        <v>25</v>
+      </c>
       <c r="D20" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="21" t="s">
-        <v>93</v>
+      <c r="E20" s="18" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="34"/>
-      <c r="B21" s="12" t="s">
+      <c r="A21" s="24"/>
+      <c r="B21" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="14" t="s">
+      <c r="C21" s="10">
+        <v>4</v>
+      </c>
+      <c r="D21" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="15" t="s">
-        <v>57</v>
+      <c r="E21" s="12" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="33" t="s">
+      <c r="A22" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="6">
         <v>1</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="11"/>
+      <c r="E22" s="8"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="35"/>
+      <c r="A23" s="25"/>
       <c r="B23" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="4"/>
+      <c r="C23" s="4">
+        <v>330</v>
+      </c>
       <c r="D23" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="21" t="s">
-        <v>91</v>
+      <c r="E23" s="18" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="35"/>
+      <c r="A24" s="25"/>
       <c r="B24" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="4"/>
+      <c r="C24" s="26">
+        <v>-1E-3</v>
+      </c>
       <c r="D24" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E24" s="21" t="s">
-        <v>90</v>
+      <c r="E24" s="18" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="35"/>
+      <c r="A25" s="25"/>
       <c r="B25" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="4"/>
+      <c r="C25" s="4">
+        <v>2</v>
+      </c>
       <c r="D25" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E25" s="21" t="s">
-        <v>89</v>
+      <c r="E25" s="18" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="35"/>
+      <c r="A26" s="25"/>
       <c r="B26" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="4"/>
+      <c r="C26" s="4">
+        <v>250</v>
+      </c>
       <c r="D26" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E26" s="21" t="s">
-        <v>88</v>
+      <c r="E26" s="18" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="35"/>
+      <c r="A27" s="25"/>
       <c r="B27" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="4"/>
+      <c r="C27" s="26">
+        <v>1E-4</v>
+      </c>
       <c r="D27" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E27" s="21" t="s">
-        <v>82</v>
+      <c r="E27" s="18" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="35"/>
+      <c r="A28" s="25"/>
       <c r="B28" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="4"/>
+      <c r="C28" s="4">
+        <v>2</v>
+      </c>
       <c r="D28" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E28" s="21" t="s">
-        <v>89</v>
+      <c r="E28" s="18" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="35"/>
+      <c r="A29" s="25"/>
       <c r="B29" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="4"/>
+      <c r="C29" s="4">
+        <v>250</v>
+      </c>
       <c r="D29" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E29" s="21" t="s">
-        <v>88</v>
+      <c r="E29" s="18" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="35"/>
+      <c r="A30" s="25"/>
       <c r="B30" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="4"/>
+      <c r="C30" s="26">
+        <v>1E-4</v>
+      </c>
       <c r="D30" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E30" s="21" t="s">
-        <v>82</v>
+      <c r="E30" s="18" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="35"/>
+      <c r="A31" s="25"/>
       <c r="B31" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C31" s="4"/>
+      <c r="C31" s="4">
+        <v>800</v>
+      </c>
       <c r="D31" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E31" s="21" t="s">
-        <v>81</v>
+      <c r="E31" s="18" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="34"/>
-      <c r="B32" s="12" t="s">
+      <c r="A32" s="24"/>
+      <c r="B32" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="14" t="s">
+      <c r="C32" s="10">
+        <v>1000</v>
+      </c>
+      <c r="D32" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E32" s="15" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C33" s="9">
-        <v>1</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E33" s="11"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="35"/>
-      <c r="B34" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E34" s="21" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="34"/>
-      <c r="B35" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="C35" s="22"/>
-      <c r="D35" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="E35" s="15" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C36" s="9"/>
-      <c r="D36" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E36" s="11"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="31"/>
-      <c r="B37" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="E37" s="29" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="31"/>
-      <c r="B38" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C38" s="6"/>
-      <c r="D38" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E38" s="29" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="31"/>
-      <c r="B39" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C39" s="6"/>
-      <c r="D39" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E39" s="29" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="31"/>
-      <c r="B40" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E40" s="29" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="31"/>
-      <c r="B41" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E41" s="21" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="31"/>
-      <c r="B42" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C42" s="4"/>
-      <c r="D42" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E42" s="21"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="31"/>
-      <c r="B43" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="C43" s="4"/>
-      <c r="D43" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E43" s="21"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="31"/>
-      <c r="B44" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C44" s="4"/>
-      <c r="D44" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E44" s="21"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="31"/>
-      <c r="B45" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="C45" s="4"/>
-      <c r="D45" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E45" s="21"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="31"/>
-      <c r="B46" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="C46" s="4"/>
-      <c r="D46" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E46" s="21"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="31"/>
-      <c r="B47" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="C47" s="4"/>
-      <c r="D47" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E47" s="21"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="31"/>
-      <c r="B48" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="C48" s="4"/>
-      <c r="D48" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E48" s="21"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="31"/>
-      <c r="B49" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="C49" s="4"/>
-      <c r="D49" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E49" s="21"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="31"/>
-      <c r="B50" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="C50" s="4"/>
-      <c r="D50" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E50" s="21"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="31"/>
-      <c r="B51" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="C51" s="4"/>
-      <c r="D51" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E51" s="21"/>
-    </row>
-    <row r="52" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="32"/>
-      <c r="B52" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="C52" s="13"/>
-      <c r="D52" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="E52" s="15"/>
+      <c r="E32" s="12" t="s">
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A36:A52"/>
+  <mergeCells count="5">
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A8:A14"/>
     <mergeCell ref="A15:A21"/>
     <mergeCell ref="A22:A32"/>
-    <mergeCell ref="A33:A35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1678,7 +1320,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>